<commit_message>
Minor edits on calibration data
</commit_message>
<xml_diff>
--- a/irCalibration.xlsx
+++ b/irCalibration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Voltage</t>
   </si>
@@ -34,16 +34,13 @@
     <t>Distance</t>
   </si>
   <si>
-    <t xml:space="preserve">IR Sensor: </t>
+    <t>2D120X</t>
   </si>
   <si>
-    <t>Green signal wire</t>
+    <t>Dark green signal wire</t>
   </si>
   <si>
-    <t>Long Vcc</t>
-  </si>
-  <si>
-    <t>"double" wires</t>
+    <t>Light green 2Y0A21</t>
   </si>
 </sst>
 </file>
@@ -187,7 +184,43 @@
             </c:spPr>
             <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5931758530183728E-2"/>
+                  <c:y val="-0.12493474773986585"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -295,11 +328,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360631496"/>
-        <c:axId val="360628360"/>
+        <c:axId val="195400920"/>
+        <c:axId val="195862360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360631496"/>
+        <c:axId val="195400920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,12 +389,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360628360"/>
+        <c:crossAx val="195862360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360628360"/>
+        <c:axId val="195862360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,7 +451,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360631496"/>
+        <c:crossAx val="195400920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -555,7 +588,43 @@
             </c:spPr>
             <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.2120078740157482E-2"/>
+                  <c:y val="-0.11577500729075532"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -663,11 +732,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="365053912"/>
-        <c:axId val="365057440"/>
+        <c:axId val="195865888"/>
+        <c:axId val="195867456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="365053912"/>
+        <c:axId val="195865888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,12 +793,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365057440"/>
+        <c:crossAx val="195867456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="365057440"/>
+        <c:axId val="195867456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365053912"/>
+        <c:crossAx val="195865888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -923,7 +992,43 @@
             </c:spPr>
             <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11487248468941383"/>
+                  <c:y val="-7.9454651501895592E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1031,11 +1136,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="365052736"/>
-        <c:axId val="365052344"/>
+        <c:axId val="195865104"/>
+        <c:axId val="195860792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="365052736"/>
+        <c:axId val="195865104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,12 +1197,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365052344"/>
+        <c:crossAx val="195860792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="365052344"/>
+        <c:axId val="195860792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1154,7 +1259,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365052736"/>
+        <c:crossAx val="195865104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3241,8 +3346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3289,9 +3394,6 @@
       <c r="B5" s="1">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -3396,10 +3498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3516,9 +3618,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>4</v>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3529,7 +3631,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -3649,9 +3751,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>5</v>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>